<commit_message>
data process error message, region
</commit_message>
<xml_diff>
--- a/data-raw/model-runs/BR_voluntarysupplement_2023.xlsx
+++ b/data-raw/model-runs/BR_voluntarysupplement_2023.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbrownin\GitHub\BTR\data-raw\model-runs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dlopez\Github\BTR\data-raw\model-runs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF60E05-FF5C-4504-98F7-2C8B62DEFA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41F8F9D-7360-41BC-B389-3F239E77EEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{5D257420-CEFD-4359-9AD1-E1CEE4FC7F7A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{5D257420-CEFD-4359-9AD1-E1CEE4FC7F7A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="br_vs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -564,7 +564,7 @@
   <dimension ref="A1:M170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>